<commit_message>
Separating the formatting from the actual scripting.
</commit_message>
<xml_diff>
--- a/glucoseReadings.xlsx
+++ b/glucoseReadings.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabiol\Documents\Studies\insights-blood-glucose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E66E74-0C09-47CC-AC9D-0BCAF1A697A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BCB882-1C1C-4934-87AE-383678D208A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5955" windowWidth="29040" windowHeight="15840" xr2:uid="{B067E57B-9BDD-4F7F-BCE4-28D96B13C186}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="_" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -86,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,16 +109,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28D9F08-A0C5-4EF7-A339-6E8C877F1113}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,25 +466,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1001,6 +1015,121 @@
       </c>
       <c r="G24" s="4">
         <v>5.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>44218</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="F25" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G25" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>44219</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="F26" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G26" s="2">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>44220</v>
+      </c>
+      <c r="B27" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G27" s="2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>44221</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="D28" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F28" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G28" s="2">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>44222</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C29" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="F29" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G29" s="2">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidied the sources; functionality unchanged.
</commit_message>
<xml_diff>
--- a/glucoseReadings.xlsx
+++ b/glucoseReadings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabiol\Documents\Studies\insights-blood-glucose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BCB882-1C1C-4934-87AE-383678D208A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4854C543-CFA7-407D-902E-54E150BE4781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5955" windowWidth="29040" windowHeight="15840" xr2:uid="{B067E57B-9BDD-4F7F-BCE4-28D96B13C186}"/>
   </bookViews>
@@ -447,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28D9F08-A0C5-4EF7-A339-6E8C877F1113}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A30" sqref="A30:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,6 +1132,52 @@
         <v>4.5</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>44223</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C30" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="F30" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>44224</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C31" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="F31" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G31" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>